<commit_message>
Add numriec 1 field test
</commit_message>
<xml_diff>
--- a/Project/True/Data Platform Naming Conventions_V1.0.5.xlsx
+++ b/Project/True/Data Platform Naming Conventions_V1.0.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://truecorp.sharepoint.com/sites/ITDataPlatform/Shared Documents/Design Document/03. Naming Convention/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWIFT\Documents\Truecrop\Project\True\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BFBD402-41E2-444D-A938-3A5F0545191A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FEF06D-DB8D-4DBB-8898-E86533C9FBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15720" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="21" r:id="rId1"/>
@@ -10555,12 +10555,12 @@
   <cellStyles count="9">
     <cellStyle name="Explanatory Text 2" xfId="4" xr:uid="{021EBAB7-F2FC-4272-A9C2-BD5738D4E571}"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{09EA258D-9B28-4C66-BFB2-85D26199ED59}"/>
     <cellStyle name="Normal 2 2" xfId="5" xr:uid="{3E3EA2FB-B864-4F5D-B5DE-990AC8779D88}"/>
     <cellStyle name="Normal 3" xfId="7" xr:uid="{919F6084-5A77-43CE-866B-D04399CD412A}"/>
     <cellStyle name="Normal 4" xfId="6" xr:uid="{77975EF8-9DDF-4556-A44F-85FB05227198}"/>
     <cellStyle name="Normal 8" xfId="2" xr:uid="{1583D981-113C-4BF8-B80B-7D74ACCC7E99}"/>
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
     <cellStyle name="ปกติ 2" xfId="8" xr:uid="{C14B9233-B70E-43EC-BBAC-A660076D8DDD}"/>
   </cellStyles>
   <dxfs count="7">
@@ -11506,11 +11506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A332B7C-D4FB-4158-8BE7-917D9FEB5BDF}">
-  <dimension ref="A2:G64"/>
+  <dimension ref="A2:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="13.5"/>
@@ -12578,6 +12578,11 @@
         <v>64</v>
       </c>
       <c r="G64" s="252"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="56">
+        <v>1111111111</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
@@ -13893,7 +13898,7 @@
       <c r="O64" s="88"/>
       <c r="U64"/>
     </row>
-    <row r="65" spans="1:15" ht="25.5">
+    <row r="65" spans="1:15" ht="27">
       <c r="A65" s="161" t="s">
         <v>254</v>
       </c>
@@ -14580,8 +14585,8 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A463" sqref="A463"/>
-      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -22247,7 +22252,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="415" spans="1:6" ht="27">
+    <row r="415" spans="1:6" ht="40.5">
       <c r="A415" s="133" t="s">
         <v>1173</v>
       </c>
@@ -22307,7 +22312,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="13.5">
+    <row r="418" spans="1:6" ht="27">
       <c r="A418" s="133" t="s">
         <v>1180</v>
       </c>
@@ -22327,7 +22332,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="13.5">
+    <row r="419" spans="1:6" ht="27">
       <c r="A419" s="133" t="s">
         <v>1182</v>
       </c>
@@ -22347,7 +22352,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="13.5">
+    <row r="420" spans="1:6" ht="27">
       <c r="A420" s="133" t="s">
         <v>1184</v>
       </c>
@@ -22367,7 +22372,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="421" spans="1:6" ht="13.5">
+    <row r="421" spans="1:6" ht="40.5">
       <c r="A421" s="133" t="s">
         <v>1186</v>
       </c>
@@ -22387,7 +22392,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="27">
+    <row r="422" spans="1:6" ht="67.5">
       <c r="A422" s="133" t="s">
         <v>1188</v>
       </c>
@@ -22407,7 +22412,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="423" spans="1:6" ht="27">
+    <row r="423" spans="1:6" ht="40.5">
       <c r="A423" s="133" t="s">
         <v>1190</v>
       </c>
@@ -22427,7 +22432,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="424" spans="1:6" ht="27">
+    <row r="424" spans="1:6" ht="40.5">
       <c r="A424" s="133" t="s">
         <v>1192</v>
       </c>
@@ -22447,7 +22452,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="425" spans="1:6" ht="27">
+    <row r="425" spans="1:6" ht="40.5">
       <c r="A425" s="133" t="s">
         <v>1194</v>
       </c>
@@ -22467,7 +22472,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="27">
+    <row r="426" spans="1:6" ht="40.5">
       <c r="A426" s="133" t="s">
         <v>1196</v>
       </c>
@@ -22487,7 +22492,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="427" spans="1:6" ht="13.5">
+    <row r="427" spans="1:6" ht="40.5">
       <c r="A427" s="133" t="s">
         <v>1198</v>
       </c>
@@ -22607,7 +22612,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="433" spans="1:6" ht="13.5">
+    <row r="433" spans="1:6" ht="27">
       <c r="A433" s="133" t="s">
         <v>1214</v>
       </c>
@@ -22627,7 +22632,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="54">
+    <row r="434" spans="1:6" ht="81">
       <c r="A434" s="262" t="s">
         <v>1217</v>
       </c>
@@ -23207,7 +23212,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="463" spans="1:6" ht="50.25">
+    <row r="463" spans="1:6" ht="54">
       <c r="A463" s="276" t="s">
         <v>1281</v>
       </c>
@@ -34036,6 +34041,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b1ddecee-520f-451d-8648-b2f1e1b31a88">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5439e425-2ef7-45b5-92f6-7784de0434bf" xsi:nil="true"/>
+    <Status xmlns="b1ddecee-520f-451d-8648-b2f1e1b31a88">Open</Status>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="เอกสาร" ma:contentTypeID="0x0101006AAEC931CD5AC046AEE6CC00CBC4A4EB" ma:contentTypeVersion="17" ma:contentTypeDescription="สร้างเอกสารใหม่" ma:contentTypeScope="" ma:versionID="8ed0ca1f33bc239db8a39eb4887baf11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b1ddecee-520f-451d-8648-b2f1e1b31a88" xmlns:ns3="5439e425-2ef7-45b5-92f6-7784de0434bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="538ae588068f00275b5fb97fe799ce85" ns2:_="" ns3:_="">
     <xsd:import namespace="b1ddecee-520f-451d-8648-b2f1e1b31a88"/>
@@ -34288,35 +34314,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b1ddecee-520f-451d-8648-b2f1e1b31a88">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5439e425-2ef7-45b5-92f6-7784de0434bf" xsi:nil="true"/>
-    <Status xmlns="b1ddecee-520f-451d-8648-b2f1e1b31a88">Open</Status>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D404CBE7-64C7-459D-8CB4-F33FE992A3F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3769-9546-4D63-B3E9-CD1BF1927AD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48272ABE-0217-457F-9489-5AF647B690A5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48272ABE-0217-457F-9489-5AF647B690A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b1ddecee-520f-451d-8648-b2f1e1b31a88"/>
+    <ds:schemaRef ds:uri="5439e425-2ef7-45b5-92f6-7784de0434bf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3769-9546-4D63-B3E9-CD1BF1927AD3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D404CBE7-64C7-459D-8CB4-F33FE992A3F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b1ddecee-520f-451d-8648-b2f1e1b31a88"/>
+    <ds:schemaRef ds:uri="5439e425-2ef7-45b5-92f6-7784de0434bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>